<commit_message>
Version Jan 31, 2022
</commit_message>
<xml_diff>
--- a/data_driven/data_preparation/input/data_preparations.xlsx
+++ b/data_driven/data_preparation/input/data_preparations.xlsx
@@ -514,27 +514,27 @@
   <dimension ref="A1:O38"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A3:A5"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.13671875" defaultRowHeight="13.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col width="9.140000000000001" customWidth="1" style="7" min="1" max="1"/>
-    <col width="12" customWidth="1" style="7" min="2" max="2"/>
+    <col width="9.130000000000001" customWidth="1" style="7" min="1" max="1"/>
+    <col width="11.99" customWidth="1" style="7" min="2" max="2"/>
     <col width="14.57" customWidth="1" style="7" min="3" max="3"/>
     <col width="13.14" customWidth="1" style="7" min="4" max="4"/>
-    <col width="15.43" customWidth="1" style="7" min="5" max="5"/>
+    <col width="15.42" customWidth="1" style="7" min="5" max="5"/>
     <col width="16.28" customWidth="1" style="7" min="6" max="6"/>
-    <col width="13.28" customWidth="1" style="7" min="7" max="7"/>
+    <col width="13.29" customWidth="1" style="7" min="7" max="7"/>
     <col width="13.43" customWidth="1" style="7" min="8" max="8"/>
     <col width="14.57" customWidth="1" style="7" min="9" max="10"/>
     <col width="15" customWidth="1" style="7" min="11" max="11"/>
-    <col width="13" customWidth="1" style="7" min="12" max="12"/>
+    <col width="13.02" customWidth="1" style="7" min="12" max="12"/>
     <col width="12.43" customWidth="1" style="7" min="13" max="13"/>
-    <col width="14" customWidth="1" style="7" min="14" max="14"/>
+    <col width="14.01" customWidth="1" style="7" min="14" max="14"/>
     <col width="18.19" customWidth="1" style="7" min="15" max="15"/>
-    <col width="9.140000000000001" customWidth="1" style="7" min="16" max="998"/>
-    <col width="9.140000000000001" customWidth="1" style="8" min="999" max="1025"/>
+    <col width="9.130000000000001" customWidth="1" style="7" min="16" max="998"/>
+    <col width="9.130000000000001" customWidth="1" style="8" min="999" max="1024"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1" s="9">

</xml_diff>

<commit_message>
Version Feb 24, 2022
</commit_message>
<xml_diff>
--- a/data_driven/data_preparation/input/data_preparations.xlsx
+++ b/data_driven/data_preparation/input/data_preparations.xlsx
@@ -513,8 +513,8 @@
   </sheetPr>
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9:A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.13671875" defaultRowHeight="13.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Version Mar 5, 2022
</commit_message>
<xml_diff>
--- a/data_driven/data_preparation/input/data_preparations.xlsx
+++ b/data_driven/data_preparation/input/data_preparations.xlsx
@@ -513,11 +513,11 @@
   </sheetPr>
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9:A38"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.13671875" defaultRowHeight="13.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.13671875" defaultRowHeight="13.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="9.130000000000001" customWidth="1" style="7" min="1" max="1"/>
     <col width="11.99" customWidth="1" style="7" min="2" max="2"/>

</xml_diff>